<commit_message>
Updated for MonoUtenza and excel ->Clients
</commit_message>
<xml_diff>
--- a/docs/tp/Clients/Clients - Conti Correnti.xlsx
+++ b/docs/tp/Clients/Clients - Conti Correnti.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TA\matrix-web-fe-tests\docs\tp\Clients\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TA\matrix-web-fe-tests\docs\tp\Clients\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51069BC2-A6EC-4796-8841-A7817CB43775}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B6BE3B2-A1FA-4E85-A1F3-17F4A44329DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-60" yWindow="-60" windowWidth="28920" windowHeight="15900" xr2:uid="{BE46A6EB-3E52-4087-BE1D-BF4A8643FA88}"/>
+    <workbookView xWindow="810" yWindow="3750" windowWidth="26235" windowHeight="12525" xr2:uid="{BE46A6EB-3E52-4087-BE1D-BF4A8643FA88}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="2" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="28">
   <si>
     <t>Design</t>
   </si>
@@ -111,6 +111,12 @@
   </si>
   <si>
     <t xml:space="preserve">Verificare che il Conto corrente sia stato eliminato correttamente nella tabella del tab Conti correnti </t>
+  </si>
+  <si>
+    <t>Matrix Web : Conti Correnti_Verifica Modifica Conto corrente</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verificare che il Conto corrente sia stato modificato correttamente nella tabella del tab Conti correnti </t>
   </si>
 </sst>
 </file>
@@ -539,10 +545,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1AEFEBA-728D-4FDD-9B3D-F6BE0E3793BC}">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD4"/>
+      <selection activeCell="J4" sqref="A4:J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -657,13 +663,13 @@
     </row>
     <row r="4" spans="1:10" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>19</v>
@@ -684,6 +690,38 @@
         <v>2</v>
       </c>
       <c r="J4" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="J5" s="3" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>